<commit_message>
improved course selection layout and added course desc and credits to recommendation
</commit_message>
<xml_diff>
--- a/project/exampleXL.xlsx
+++ b/project/exampleXL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ompatel/Desktop/fourward/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882D1CF3-F172-924A-8EAC-1745FA97CFDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3A2A57-1DCC-9941-BA9A-1CE9668304AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{99EABBEA-7796-5C47-8013-427392CF7BE4}"/>
   </bookViews>
@@ -575,7 +575,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -708,6 +708,9 @@
       <c r="B10" t="s">
         <v>3</v>
       </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
       <c r="D10" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
made getting prerequisite screen display a popup instead of being sent to another page
</commit_message>
<xml_diff>
--- a/project/exampleXL.xlsx
+++ b/project/exampleXL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ompatel/Desktop/fourward/project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3A2A57-1DCC-9941-BA9A-1CE9668304AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A18506-F003-DD43-B1A4-46745B0AE28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{99EABBEA-7796-5C47-8013-427392CF7BE4}"/>
   </bookViews>
@@ -572,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{391E73AB-77E2-084D-9D4C-C3E7CDC41DE6}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,171 +729,171 @@
         <v>35</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="C14">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" t="s">
         <v>27</v>
       </c>
-      <c r="B21" t="s">
-        <v>50</v>
-      </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24">
-        <v>3</v>
-      </c>
-      <c r="D24" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>